<commit_message>
Update AIL and Timeline
</commit_message>
<xml_diff>
--- a/Logistics/AIL_75_JPB_Fall.xlsx
+++ b/Logistics/AIL_75_JPB_Fall.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>Team Members:</t>
   </si>
@@ -151,6 +151,27 @@
   </si>
   <si>
     <t>Get Projector</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>"Casey is bad at script writing" - Casey</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Waiting on profs</t>
+  </si>
+  <si>
+    <t>Late</t>
+  </si>
+  <si>
+    <t>On Hold</t>
+  </si>
+  <si>
+    <t>Waiting for Prezi and Script</t>
   </si>
 </sst>
 </file>
@@ -703,35 +724,6 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <numFmt numFmtId="0" formatCode="yyyy\-mm\-dd;@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -806,6 +798,35 @@
       </fill>
       <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -820,20 +841,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A13:H77" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A13:H77" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A13:H77"/>
   <sortState ref="A14:H77">
     <sortCondition ref="D13:D77"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="#" dataDxfId="9"/>
-    <tableColumn id="3" name="Activity" dataDxfId="8"/>
-    <tableColumn id="4" name="Person(s)" dataDxfId="7"/>
-    <tableColumn id="5" name="Date Assigned" dataDxfId="6"/>
-    <tableColumn id="6" name="Date Due" dataDxfId="5"/>
-    <tableColumn id="7" name="New Due" dataDxfId="4"/>
-    <tableColumn id="8" name="Status" dataDxfId="3"/>
-    <tableColumn id="9" name="Comments" dataDxfId="2"/>
+    <tableColumn id="1" name="#" dataDxfId="7"/>
+    <tableColumn id="3" name="Activity" dataDxfId="6"/>
+    <tableColumn id="4" name="Person(s)" dataDxfId="5"/>
+    <tableColumn id="5" name="Date Assigned" dataDxfId="4"/>
+    <tableColumn id="6" name="Date Due" dataDxfId="3"/>
+    <tableColumn id="7" name="New Due" dataDxfId="2"/>
+    <tableColumn id="8" name="Status" dataDxfId="1"/>
+    <tableColumn id="9" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1128,8 +1149,8 @@
   </sheetPr>
   <dimension ref="A1:KS78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1864,7 +1885,9 @@
         <v>41879</v>
       </c>
       <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
+      <c r="G14" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
       <c r="J14" s="21"/>
@@ -2180,9 +2203,15 @@
       <c r="E15" s="9">
         <v>41879</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="21"/>
+      <c r="F15" s="9">
+        <v>41880</v>
+      </c>
+      <c r="G15" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="16" spans="1:305" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="21">
@@ -2201,7 +2230,9 @@
         <v>41884</v>
       </c>
       <c r="F16" s="9"/>
-      <c r="G16" s="10"/>
+      <c r="G16" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
       <c r="J16" s="21"/>
@@ -2537,8 +2568,12 @@
       <c r="E18" s="9">
         <v>41879</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="10"/>
+      <c r="F18" s="9">
+        <v>41885</v>
+      </c>
+      <c r="G18" s="13">
+        <v>0</v>
+      </c>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
       <c r="J18" s="21"/>
@@ -3212,7 +3247,9 @@
         <v>41879</v>
       </c>
       <c r="F22" s="9"/>
-      <c r="G22" s="10"/>
+      <c r="G22" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="H22" s="21"/>
       <c r="I22" s="21"/>
       <c r="J22" s="21"/>
@@ -3529,8 +3566,12 @@
         <v>41878</v>
       </c>
       <c r="F23" s="9"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="21"/>
+      <c r="G23" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="24" spans="1:305" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="21">
@@ -3549,8 +3590,12 @@
         <v>41878</v>
       </c>
       <c r="F24" s="9"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="21"/>
+      <c r="G24" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>50</v>
+      </c>
       <c r="I24" s="21"/>
       <c r="J24" s="21"/>
       <c r="K24" s="21"/>
@@ -3866,7 +3911,9 @@
         <v>41878</v>
       </c>
       <c r="F25" s="9"/>
-      <c r="G25" s="10"/>
+      <c r="G25" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="H25" s="21"/>
     </row>
     <row r="26" spans="1:305" s="24" customFormat="1" x14ac:dyDescent="0.2">
@@ -4215,8 +4262,12 @@
         <v>41879</v>
       </c>
       <c r="F28" s="9"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="25"/>
+      <c r="G28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="29" spans="1:305" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="21">

</xml_diff>

<commit_message>
Add Wk7 Report and update AIL
</commit_message>
<xml_diff>
--- a/Logistics/AIL_75_JPB_Fall.xlsx
+++ b/Logistics/AIL_75_JPB_Fall.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="123820"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\GitHub\SeniorDesign\Logistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chance\Documents\GitHub\SeniorDesign\Logistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="89">
   <si>
     <t>Team Members:</t>
   </si>
@@ -1260,8 +1260,8 @@
   </sheetPr>
   <dimension ref="A1:KS86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6679,8 +6679,8 @@
       <c r="F50" s="9">
         <v>41905</v>
       </c>
-      <c r="G50" s="13">
-        <v>0.25</v>
+      <c r="G50" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="H50" s="20"/>
     </row>
@@ -7018,7 +7018,9 @@
         <v>41921</v>
       </c>
       <c r="F52" s="9"/>
-      <c r="G52" s="10"/>
+      <c r="G52" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="H52" s="20"/>
     </row>
     <row r="53" spans="1:305" s="23" customFormat="1" x14ac:dyDescent="0.2">
@@ -7038,7 +7040,9 @@
         <v>41912</v>
       </c>
       <c r="F53" s="9"/>
-      <c r="G53" s="10"/>
+      <c r="G53" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="H53" s="20"/>
       <c r="I53" s="20"/>
       <c r="J53" s="20"/>
@@ -7374,8 +7378,12 @@
       <c r="E55" s="9">
         <v>41914</v>
       </c>
-      <c r="F55" s="9"/>
-      <c r="G55" s="10"/>
+      <c r="F55" s="9">
+        <v>41928</v>
+      </c>
+      <c r="G55" s="13">
+        <v>0.4</v>
+      </c>
       <c r="H55" s="20"/>
       <c r="I55" s="20"/>
       <c r="J55" s="20"/>

</xml_diff>